<commit_message>
modified the excel file to ensure better data retrieval in pandas using read_excel method
</commit_message>
<xml_diff>
--- a/etl_processor/data_source/energy/ElectricityGenerationAndConsumption.xlsx
+++ b/etl_processor/data_source/energy/ElectricityGenerationAndConsumption.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BB285F-9BF8-324B-B70A-55A9E60F0243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED54830-78A8-9947-9EA4-FE4A1264DEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63460" yWindow="7100" windowWidth="51200" windowHeight="27060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46320" yWindow="1160" windowWidth="51200" windowHeight="27060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M890841" sheetId="1" r:id="rId1"/>
@@ -321,6 +321,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -715,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD52"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AW55" sqref="AW55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -911,81 +912,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:50" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="AW11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AX11" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="AW12" s="5">
-        <v>4604.8999999999996</v>
-      </c>
-      <c r="AX12" s="5">
-        <v>4175.7</v>
-      </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>79</v>
       </c>
-      <c r="AW13" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX13" s="5" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>80</v>
       </c>
-      <c r="AW14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX14" s="5" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>81</v>
       </c>
-      <c r="AW15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX15" s="5" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>82</v>
       </c>
-      <c r="AW16" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX16" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="AW17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX17" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>83</v>
       </c>
@@ -994,138 +951,64 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="AW18" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX18" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>84</v>
       </c>
-      <c r="AW19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX19" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>85</v>
       </c>
-      <c r="AW20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX20" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>86</v>
       </c>
-      <c r="AW21" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX21" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>87</v>
       </c>
-      <c r="AW22" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX22" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
-      <c r="AW23" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX23" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>89</v>
       </c>
-      <c r="AW24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX24" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>90</v>
       </c>
-      <c r="AW25" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX25" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>91</v>
       </c>
-      <c r="AW26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX26" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="AW27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX27" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>92</v>
       </c>
-      <c r="AW28" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX28" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>93</v>
       </c>
-      <c r="AW29" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX29" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:48" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:50" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>8</v>
       </c>
@@ -1270,8 +1153,14 @@
       <c r="AV34" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX34" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>58</v>
       </c>
@@ -1416,8 +1305,14 @@
       <c r="AV35" s="5">
         <v>5114.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW35" s="5">
+        <v>4604.8999999999996</v>
+      </c>
+      <c r="AX35" s="5">
+        <v>4175.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>59</v>
       </c>
@@ -1562,8 +1457,14 @@
       <c r="AV36" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW36" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX36" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>61</v>
       </c>
@@ -1708,8 +1609,14 @@
       <c r="AV37" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX37" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>62</v>
       </c>
@@ -1854,8 +1761,14 @@
       <c r="AV38" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX38" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>63</v>
       </c>
@@ -2000,8 +1913,14 @@
       <c r="AV39" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW39" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX39" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>64</v>
       </c>
@@ -2146,8 +2065,14 @@
       <c r="AV40" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX40" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>65</v>
       </c>
@@ -2292,8 +2217,14 @@
       <c r="AV41" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW41" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX41" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>66</v>
       </c>
@@ -2438,8 +2369,14 @@
       <c r="AV42" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW42" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX42" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>67</v>
       </c>
@@ -2584,8 +2521,14 @@
       <c r="AV43" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX43" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>68</v>
       </c>
@@ -2730,8 +2673,14 @@
       <c r="AV44" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW44" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX44" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>69</v>
       </c>
@@ -2876,8 +2825,14 @@
       <c r="AV45" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW45" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX45" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>70</v>
       </c>
@@ -3022,8 +2977,14 @@
       <c r="AV46" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW46" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX46" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>71</v>
       </c>
@@ -3168,8 +3129,14 @@
       <c r="AV47" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW47" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX47" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>72</v>
       </c>
@@ -3314,8 +3281,14 @@
       <c r="AV48" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW48" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX48" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>73</v>
       </c>
@@ -3460,8 +3433,14 @@
       <c r="AV49" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW49" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX49" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>74</v>
       </c>
@@ -3606,8 +3585,14 @@
       <c r="AV50" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW50" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX50" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>75</v>
       </c>
@@ -3752,8 +3737,14 @@
       <c r="AV51" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW51" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX51" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>76</v>
       </c>
@@ -3896,6 +3887,12 @@
         <v>60</v>
       </c>
       <c r="AV52" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW52" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX52" s="5" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>